<commit_message>
Add testschedule with Opera tests
</commit_message>
<xml_diff>
--- a/assets/documents/excelfiles/testsheet.xlsx
+++ b/assets/documents/excelfiles/testsheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richardread/Dropbox (Personal)/WebPages/CodeInstitute/Milestone Project 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richardread/Dropbox (Personal)/WebPages/CodeInstitute/Milestone Project 2/TestSchedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1531073-6A27-9041-BF6B-889F8F544570}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E6BA4D-E1FC-F641-BE0B-695C9DCA078D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{B60DCFBD-456B-3146-8D00-48723182578D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20520" xr2:uid="{B60DCFBD-456B-3146-8D00-48723182578D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="56">
   <si>
     <t>Chrome</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>Not Tested</t>
+  </si>
+  <si>
+    <t>Opera</t>
   </si>
 </sst>
 </file>
@@ -403,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -468,15 +471,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -499,6 +493,24 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -815,11 +827,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54BB2D18-418D-6D4D-B342-24E65D184D70}">
-  <dimension ref="A1:G124"/>
+  <dimension ref="A1:H124"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I70" sqref="I70"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K115" sqref="K115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -829,61 +841,66 @@
     <col min="3" max="3" width="12.83203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="14.1640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="13" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="7" width="12.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="23"/>
-    </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="35"/>
+    </row>
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>50</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="22"/>
+      <c r="H2" s="30" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>48</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="31"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
@@ -905,8 +922,11 @@
       <c r="G4" s="14" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="11" t="s">
         <v>26</v>
@@ -926,8 +946,11 @@
       <c r="G5" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="11" t="s">
         <v>27</v>
@@ -947,8 +970,11 @@
       <c r="G6" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
       <c r="B7" s="11" t="s">
         <v>9</v>
@@ -968,8 +994,11 @@
       <c r="G7" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="11" t="s">
         <v>10</v>
@@ -989,8 +1018,11 @@
       <c r="G8" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
       <c r="B9" s="11" t="s">
         <v>11</v>
@@ -1010,8 +1042,11 @@
       <c r="G9" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="11" t="s">
         <v>12</v>
@@ -1031,8 +1066,11 @@
       <c r="G10" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
       <c r="B11" s="11" t="s">
         <v>13</v>
@@ -1052,8 +1090,11 @@
       <c r="G11" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="11" t="s">
         <v>14</v>
@@ -1073,8 +1114,11 @@
       <c r="G12" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
       <c r="B13" s="11" t="s">
         <v>15</v>
@@ -1091,11 +1135,14 @@
       <c r="F13" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="31" t="s">
+      <c r="G13" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="11" t="s">
         <v>46</v>
@@ -1112,11 +1159,14 @@
       <c r="F14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
       <c r="B15" s="11" t="s">
         <v>16</v>
@@ -1133,11 +1183,14 @@
       <c r="F15" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="11" t="s">
         <v>17</v>
@@ -1154,11 +1207,14 @@
       <c r="F16" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="31" t="s">
+      <c r="G16" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
       <c r="B17" s="11" t="s">
         <v>45</v>
@@ -1175,11 +1231,14 @@
       <c r="F17" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="31" t="s">
+      <c r="G17" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
       <c r="B18" s="11" t="s">
         <v>18</v>
@@ -1196,11 +1255,14 @@
       <c r="F18" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="31" t="s">
+      <c r="G18" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>
       <c r="B19" s="11" t="s">
         <v>19</v>
@@ -1217,11 +1279,14 @@
       <c r="F19" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G19" s="31" t="s">
+      <c r="G19" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="11" t="s">
         <v>20</v>
@@ -1238,11 +1303,14 @@
       <c r="F20" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G20" s="31" t="s">
+      <c r="G20" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
       <c r="B21" s="11" t="s">
         <v>21</v>
@@ -1262,8 +1330,11 @@
       <c r="G21" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H21" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="11" t="s">
         <v>22</v>
@@ -1283,8 +1354,11 @@
       <c r="G22" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H22" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
       <c r="B23" s="11" t="s">
         <v>30</v>
@@ -1304,8 +1378,11 @@
       <c r="G23" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H23" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="B24" s="11" t="s">
         <v>32</v>
@@ -1325,8 +1402,11 @@
       <c r="G24" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H24" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
       <c r="B25" s="12" t="s">
         <v>31</v>
@@ -1346,8 +1426,11 @@
       <c r="G25" s="16" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H25" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
         <v>7</v>
       </c>
@@ -1366,11 +1449,14 @@
       <c r="F26" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G26" s="32" t="s">
+      <c r="G26" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H26" s="29" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="8"/>
       <c r="B27" s="11" t="s">
         <v>23</v>
@@ -1390,8 +1476,11 @@
       <c r="G27" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H27" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="11" t="s">
         <v>28</v>
@@ -1411,8 +1500,11 @@
       <c r="G28" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H28" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="8"/>
       <c r="B29" s="11" t="s">
         <v>26</v>
@@ -1432,8 +1524,11 @@
       <c r="G29" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H29" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
       <c r="B30" s="11" t="s">
         <v>9</v>
@@ -1453,8 +1548,11 @@
       <c r="G30" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H30" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="8"/>
       <c r="B31" s="11" t="s">
         <v>10</v>
@@ -1471,11 +1569,14 @@
       <c r="F31" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G31" s="31" t="s">
+      <c r="G31" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H31" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="8"/>
       <c r="B32" s="11" t="s">
         <v>11</v>
@@ -1492,11 +1593,14 @@
       <c r="F32" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G32" s="31" t="s">
+      <c r="G32" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H32" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
       <c r="B33" s="11" t="s">
         <v>53</v>
@@ -1513,11 +1617,14 @@
       <c r="F33" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G33" s="31" t="s">
+      <c r="G33" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H33" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
       <c r="B34" s="11" t="s">
         <v>13</v>
@@ -1534,11 +1641,14 @@
       <c r="F34" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G34" s="31" t="s">
+      <c r="G34" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H34" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="8"/>
       <c r="B35" s="11" t="s">
         <v>14</v>
@@ -1555,11 +1665,14 @@
       <c r="F35" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G35" s="31" t="s">
+      <c r="G35" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H35" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="8"/>
       <c r="B36" s="11" t="s">
         <v>15</v>
@@ -1576,11 +1689,14 @@
       <c r="F36" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G36" s="31" t="s">
+      <c r="G36" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H36" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="8"/>
       <c r="B37" s="11" t="s">
         <v>46</v>
@@ -1597,11 +1713,14 @@
       <c r="F37" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G37" s="31" t="s">
+      <c r="G37" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H37" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="8"/>
       <c r="B38" s="11" t="s">
         <v>16</v>
@@ -1618,11 +1737,14 @@
       <c r="F38" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G38" s="31" t="s">
+      <c r="G38" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H38" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="8"/>
       <c r="B39" s="11" t="s">
         <v>17</v>
@@ -1639,11 +1761,14 @@
       <c r="F39" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G39" s="31" t="s">
+      <c r="G39" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H39" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="8"/>
       <c r="B40" s="11" t="s">
         <v>45</v>
@@ -1660,11 +1785,14 @@
       <c r="F40" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G40" s="31" t="s">
+      <c r="G40" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H40" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="8"/>
       <c r="B41" s="11" t="s">
         <v>18</v>
@@ -1681,11 +1809,14 @@
       <c r="F41" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G41" s="31" t="s">
+      <c r="G41" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H41" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="8"/>
       <c r="B42" s="11" t="s">
         <v>19</v>
@@ -1702,11 +1833,14 @@
       <c r="F42" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="31" t="s">
+      <c r="G42" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H42" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="8"/>
       <c r="B43" s="11" t="s">
         <v>20</v>
@@ -1723,11 +1857,14 @@
       <c r="F43" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G43" s="31" t="s">
+      <c r="G43" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H43" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="8"/>
       <c r="B44" s="11" t="s">
         <v>39</v>
@@ -1747,8 +1884,11 @@
       <c r="G44" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H44" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="8"/>
       <c r="B45" s="11" t="s">
         <v>22</v>
@@ -1768,8 +1908,11 @@
       <c r="G45" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H45" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="8"/>
       <c r="B46" s="11" t="s">
         <v>30</v>
@@ -1789,8 +1932,11 @@
       <c r="G46" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H46" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="8"/>
       <c r="B47" s="11" t="s">
         <v>32</v>
@@ -1810,8 +1956,11 @@
       <c r="G47" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H47" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="9"/>
       <c r="B48" s="12" t="s">
         <v>31</v>
@@ -1828,11 +1977,14 @@
       <c r="F48" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="G48" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G48" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H48" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="13" t="s">
         <v>29</v>
       </c>
@@ -1854,8 +2006,11 @@
       <c r="G49" s="14" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H49" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="8"/>
       <c r="B50" s="11" t="s">
         <v>23</v>
@@ -1875,8 +2030,11 @@
       <c r="G50" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H50" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="8"/>
       <c r="B51" s="11" t="s">
         <v>41</v>
@@ -1896,8 +2054,11 @@
       <c r="G51" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H51" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="8"/>
       <c r="B52" s="11" t="s">
         <v>26</v>
@@ -1917,8 +2078,11 @@
       <c r="G52" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H52" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="8"/>
       <c r="B53" s="11" t="s">
         <v>9</v>
@@ -1938,8 +2102,11 @@
       <c r="G53" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H53" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="8"/>
       <c r="B54" s="11" t="s">
         <v>49</v>
@@ -1956,11 +2123,14 @@
       <c r="F54" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G54" s="31" t="s">
+      <c r="G54" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H54" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="8"/>
       <c r="B55" s="11" t="s">
         <v>21</v>
@@ -1980,8 +2150,11 @@
       <c r="G55" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H55" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="8"/>
       <c r="B56" s="11" t="s">
         <v>40</v>
@@ -2001,8 +2174,11 @@
       <c r="G56" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H56" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="8"/>
       <c r="B57" s="11" t="s">
         <v>30</v>
@@ -2022,8 +2198,11 @@
       <c r="G57" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H57" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="8"/>
       <c r="B58" s="11" t="s">
         <v>32</v>
@@ -2043,8 +2222,11 @@
       <c r="G58" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H58" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="9"/>
       <c r="B59" s="12" t="s">
         <v>31</v>
@@ -2064,44 +2246,51 @@
       <c r="G59" s="16" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H59" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="20" t="s">
         <v>44</v>
       </c>
       <c r="B60" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C60" s="25" t="s">
+      <c r="C60" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="D60" s="25" t="s">
+      <c r="D60" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="E60" s="25" t="s">
+      <c r="E60" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="F60" s="25" t="s">
+      <c r="F60" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="G60" s="30" t="s">
+      <c r="G60" s="27"/>
+      <c r="H60" s="32" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="21" t="s">
         <v>48</v>
       </c>
       <c r="B61" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C61" s="26"/>
-      <c r="D61" s="26"/>
-      <c r="E61" s="26"/>
-      <c r="F61" s="26"/>
-      <c r="G61" s="30"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C61" s="31"/>
+      <c r="D61" s="31"/>
+      <c r="E61" s="31"/>
+      <c r="F61" s="31"/>
+      <c r="G61" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="H61" s="32"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
         <v>8</v>
       </c>
@@ -2117,14 +2306,17 @@
       <c r="E62" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="F62" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="G62" s="17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F62" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G62" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="H62" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="7"/>
       <c r="B63" s="11" t="s">
         <v>26</v>
@@ -2138,14 +2330,17 @@
       <c r="E63" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F63" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G63" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F63" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G63" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H63" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="7"/>
       <c r="B64" s="11" t="s">
         <v>37</v>
@@ -2159,14 +2354,17 @@
       <c r="E64" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F64" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G64" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F64" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G64" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H64" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="7"/>
       <c r="B65" s="11" t="s">
         <v>38</v>
@@ -2180,14 +2378,17 @@
       <c r="E65" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F65" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G65" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F65" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G65" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H65" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="7"/>
       <c r="B66" s="11" t="s">
         <v>42</v>
@@ -2201,14 +2402,17 @@
       <c r="E66" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F66" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G66" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F66" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G66" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H66" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="8"/>
       <c r="B67" s="11" t="s">
         <v>9</v>
@@ -2222,14 +2426,17 @@
       <c r="E67" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F67" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G67" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F67" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G67" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H67" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="8"/>
       <c r="B68" s="11" t="s">
         <v>10</v>
@@ -2243,14 +2450,17 @@
       <c r="E68" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F68" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G68" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F68" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G68" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H68" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="8"/>
       <c r="B69" s="11" t="s">
         <v>11</v>
@@ -2264,14 +2474,17 @@
       <c r="E69" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F69" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G69" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F69" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G69" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H69" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="8"/>
       <c r="B70" s="11" t="s">
         <v>12</v>
@@ -2285,14 +2498,17 @@
       <c r="E70" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F70" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G70" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F70" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G70" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H70" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="8"/>
       <c r="B71" s="11" t="s">
         <v>13</v>
@@ -2306,14 +2522,17 @@
       <c r="E71" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F71" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G71" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F71" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G71" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H71" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="8"/>
       <c r="B72" s="11" t="s">
         <v>14</v>
@@ -2327,14 +2546,17 @@
       <c r="E72" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F72" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G72" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F72" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G72" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H72" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="8"/>
       <c r="B73" s="11" t="s">
         <v>15</v>
@@ -2348,14 +2570,17 @@
       <c r="E73" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F73" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G73" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F73" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G73" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H73" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="8"/>
       <c r="B74" s="11" t="s">
         <v>47</v>
@@ -2369,14 +2594,17 @@
       <c r="E74" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F74" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G74" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F74" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G74" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H74" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="8"/>
       <c r="B75" s="11" t="s">
         <v>16</v>
@@ -2390,14 +2618,17 @@
       <c r="E75" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F75" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G75" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F75" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G75" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H75" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="8"/>
       <c r="B76" s="11" t="s">
         <v>17</v>
@@ -2411,14 +2642,17 @@
       <c r="E76" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F76" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G76" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F76" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G76" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H76" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="8"/>
       <c r="B77" s="11" t="s">
         <v>45</v>
@@ -2432,14 +2666,17 @@
       <c r="E77" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F77" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G77" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F77" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G77" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H77" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="8"/>
       <c r="B78" s="11" t="s">
         <v>18</v>
@@ -2453,14 +2690,17 @@
       <c r="E78" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F78" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G78" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F78" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G78" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H78" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="8"/>
       <c r="B79" s="11" t="s">
         <v>19</v>
@@ -2474,14 +2714,17 @@
       <c r="E79" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F79" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G79" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F79" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G79" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H79" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="8"/>
       <c r="B80" s="11" t="s">
         <v>20</v>
@@ -2495,14 +2738,17 @@
       <c r="E80" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F80" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G80" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F80" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G80" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H80" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="8"/>
       <c r="B81" s="11" t="s">
         <v>21</v>
@@ -2516,14 +2762,17 @@
       <c r="E81" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F81" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G81" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F81" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G81" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H81" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="8"/>
       <c r="B82" s="11" t="s">
         <v>22</v>
@@ -2537,14 +2786,17 @@
       <c r="E82" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F82" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G82" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F82" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G82" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H82" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="8"/>
       <c r="B83" s="11" t="s">
         <v>30</v>
@@ -2558,14 +2810,17 @@
       <c r="E83" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F83" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G83" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F83" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G83" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H83" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="8"/>
       <c r="B84" s="11" t="s">
         <v>32</v>
@@ -2579,14 +2834,17 @@
       <c r="E84" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F84" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G84" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F84" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G84" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H84" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="9"/>
       <c r="B85" s="12" t="s">
         <v>31</v>
@@ -2600,14 +2858,17 @@
       <c r="E85" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F85" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="G85" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F85" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G85" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="H85" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="13" t="s">
         <v>7</v>
       </c>
@@ -2623,14 +2884,17 @@
       <c r="E86" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="F86" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="G86" s="17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F86" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G86" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="H86" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="8"/>
       <c r="B87" s="11" t="s">
         <v>23</v>
@@ -2644,14 +2908,17 @@
       <c r="E87" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F87" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G87" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F87" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G87" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H87" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="8"/>
       <c r="B88" s="11" t="s">
         <v>26</v>
@@ -2665,14 +2932,17 @@
       <c r="E88" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F88" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G88" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F88" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G88" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H88" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="8"/>
       <c r="B89" s="11" t="s">
         <v>37</v>
@@ -2686,14 +2956,17 @@
       <c r="E89" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F89" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G89" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F89" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G89" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H89" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="7"/>
       <c r="B90" s="11" t="s">
         <v>38</v>
@@ -2707,14 +2980,17 @@
       <c r="E90" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F90" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G90" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F90" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G90" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H90" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="7"/>
       <c r="B91" s="11" t="s">
         <v>43</v>
@@ -2728,14 +3004,17 @@
       <c r="E91" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F91" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G91" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F91" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G91" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H91" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="8"/>
       <c r="B92" s="11" t="s">
         <v>9</v>
@@ -2749,14 +3028,17 @@
       <c r="E92" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F92" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G92" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F92" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G92" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H92" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="8"/>
       <c r="B93" s="11" t="s">
         <v>10</v>
@@ -2770,14 +3052,17 @@
       <c r="E93" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F93" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G93" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F93" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G93" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H93" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="8"/>
       <c r="B94" s="11" t="s">
         <v>11</v>
@@ -2791,14 +3076,17 @@
       <c r="E94" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F94" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G94" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F94" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G94" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H94" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="8"/>
       <c r="B95" s="11" t="s">
         <v>12</v>
@@ -2812,14 +3100,17 @@
       <c r="E95" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F95" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G95" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F95" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G95" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H95" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="8"/>
       <c r="B96" s="11" t="s">
         <v>13</v>
@@ -2833,14 +3124,17 @@
       <c r="E96" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F96" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G96" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F96" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G96" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H96" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="8"/>
       <c r="B97" s="11" t="s">
         <v>14</v>
@@ -2854,14 +3148,17 @@
       <c r="E97" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F97" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G97" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F97" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G97" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H97" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="8"/>
       <c r="B98" s="11" t="s">
         <v>15</v>
@@ -2875,14 +3172,17 @@
       <c r="E98" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F98" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G98" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F98" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G98" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H98" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="8"/>
       <c r="B99" s="11" t="s">
         <v>47</v>
@@ -2896,14 +3196,17 @@
       <c r="E99" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F99" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G99" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F99" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G99" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H99" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="8"/>
       <c r="B100" s="11" t="s">
         <v>16</v>
@@ -2917,14 +3220,17 @@
       <c r="E100" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F100" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G100" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F100" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G100" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H100" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="8"/>
       <c r="B101" s="11" t="s">
         <v>17</v>
@@ -2938,14 +3244,17 @@
       <c r="E101" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F101" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G101" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F101" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G101" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H101" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="8"/>
       <c r="B102" s="11" t="s">
         <v>45</v>
@@ -2959,14 +3268,17 @@
       <c r="E102" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F102" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G102" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F102" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G102" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H102" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="8"/>
       <c r="B103" s="11" t="s">
         <v>18</v>
@@ -2980,14 +3292,17 @@
       <c r="E103" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F103" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G103" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F103" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G103" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H103" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="8"/>
       <c r="B104" s="11" t="s">
         <v>19</v>
@@ -3001,14 +3316,17 @@
       <c r="E104" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F104" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G104" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F104" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G104" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H104" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="8"/>
       <c r="B105" s="11" t="s">
         <v>20</v>
@@ -3022,14 +3340,17 @@
       <c r="E105" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F105" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G105" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F105" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G105" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H105" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="8"/>
       <c r="B106" s="11" t="s">
         <v>39</v>
@@ -3043,14 +3364,17 @@
       <c r="E106" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F106" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G106" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F106" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G106" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H106" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="8"/>
       <c r="B107" s="11" t="s">
         <v>22</v>
@@ -3064,14 +3388,17 @@
       <c r="E107" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F107" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G107" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F107" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G107" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H107" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="8"/>
       <c r="B108" s="11" t="s">
         <v>30</v>
@@ -3085,14 +3412,17 @@
       <c r="E108" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F108" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G108" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F108" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G108" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H108" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="8"/>
       <c r="B109" s="11" t="s">
         <v>32</v>
@@ -3106,14 +3436,17 @@
       <c r="E109" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F109" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G109" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F109" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G109" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H109" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="9"/>
       <c r="B110" s="12" t="s">
         <v>31</v>
@@ -3127,14 +3460,17 @@
       <c r="E110" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F110" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="G110" s="19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F110" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G110" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="H110" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="13" t="s">
         <v>29</v>
       </c>
@@ -3153,11 +3489,14 @@
       <c r="F111" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G111" s="17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G111" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H111" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="8"/>
       <c r="B112" s="11" t="s">
         <v>23</v>
@@ -3174,11 +3513,14 @@
       <c r="F112" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G112" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G112" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H112" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="8"/>
       <c r="B113" s="11" t="s">
         <v>28</v>
@@ -3195,11 +3537,14 @@
       <c r="F113" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G113" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G113" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H113" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="8"/>
       <c r="B114" s="11" t="s">
         <v>26</v>
@@ -3216,11 +3561,14 @@
       <c r="F114" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G114" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G114" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H114" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="8"/>
       <c r="B115" s="11" t="s">
         <v>37</v>
@@ -3237,11 +3585,14 @@
       <c r="F115" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G115" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G115" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H115" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" s="8"/>
       <c r="B116" s="11" t="s">
         <v>38</v>
@@ -3258,11 +3609,14 @@
       <c r="F116" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G116" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G116" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H116" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" s="8"/>
       <c r="B117" s="11" t="s">
         <v>43</v>
@@ -3279,11 +3633,14 @@
       <c r="F117" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G117" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G117" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H117" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" s="8"/>
       <c r="B118" s="11" t="s">
         <v>9</v>
@@ -3300,11 +3657,14 @@
       <c r="F118" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G118" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G118" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H118" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="8"/>
       <c r="B119" s="11" t="s">
         <v>49</v>
@@ -3321,11 +3681,14 @@
       <c r="F119" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G119" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G119" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H119" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" s="8"/>
       <c r="B120" s="11" t="s">
         <v>21</v>
@@ -3342,11 +3705,14 @@
       <c r="F120" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G120" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G120" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H120" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="8"/>
       <c r="B121" s="11" t="s">
         <v>40</v>
@@ -3363,11 +3729,14 @@
       <c r="F121" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G121" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G121" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H121" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="8"/>
       <c r="B122" s="11" t="s">
         <v>30</v>
@@ -3384,11 +3753,14 @@
       <c r="F122" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G122" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G122" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H122" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" s="8"/>
       <c r="B123" s="11" t="s">
         <v>32</v>
@@ -3405,11 +3777,14 @@
       <c r="F123" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G123" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G123" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H123" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" s="9"/>
       <c r="B124" s="12" t="s">
         <v>31</v>
@@ -3426,24 +3801,27 @@
       <c r="F124" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="G124" s="19" t="s">
+      <c r="G124" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H124" s="19" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="F60:F61"/>
-    <mergeCell ref="G60:G61"/>
-    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="C1:H1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="H60:H61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>